<commit_message>
adds USFWS as option to drop down in template materials for funder name
</commit_message>
<xml_diff>
--- a/data-raw/metadata_template/metadata.xlsx
+++ b/data-raw/metadata_template/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\projects\EDI_CVPIA_Project\updated_EDI_materials\metadata template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/CVPIA/EMLaide/data-raw/metadata_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F024329-E48E-4438-8F8D-3901B023961D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF9DE4D-A8E0-AD47-B779-06C9A3D39E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="17580" windowHeight="8385" tabRatio="834" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -293,37 +293,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -715,20 +708,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="9" style="13"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -753,45 +746,45 @@
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.75" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="21" style="13" customWidth="1"/>
-    <col min="4" max="8" width="10.5" style="13"/>
-    <col min="9" max="9" width="10.375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="32.625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21" style="9" customWidth="1"/>
+    <col min="4" max="8" width="10.5" style="9"/>
+    <col min="9" max="9" width="10.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -810,28 +803,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.75" style="3"/>
+    <col min="1" max="2" width="19.6640625" style="3"/>
     <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.25" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="5.375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="5.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="12" customWidth="1"/>
-    <col min="9" max="9" width="14.125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="16" style="12" customWidth="1"/>
-    <col min="11" max="11" width="17.625" style="10" customWidth="1"/>
-    <col min="12" max="13" width="9.25" style="12" customWidth="1"/>
-    <col min="14" max="1021" width="19.75" style="3"/>
-    <col min="1022" max="1024" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="16" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="8" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="10" customWidth="1"/>
+    <col min="14" max="1021" width="19.6640625" style="3"/>
+    <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -841,45 +834,45 @@
       <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J2" s="11"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G10" s="15"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J2" s="9"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -912,25 +905,25 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14" style="13" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -945,14 +938,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27.375" customWidth="1"/>
-    <col min="6" max="6" width="27" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,15 +961,15 @@
       <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
     </row>
@@ -1000,13 +993,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
   </sheetData>
@@ -1031,21 +1024,21 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1060,29 +1053,29 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="13"/>
-    <col min="4" max="4" width="15.125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="26" style="13" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="9"/>
+    <col min="4" max="4" width="15.1640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1105,32 +1098,32 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9" style="13"/>
-    <col min="3" max="3" width="9" style="8"/>
-    <col min="4" max="4" width="9" style="13"/>
-    <col min="5" max="5" width="14.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="9" style="8"/>
+    <col min="1" max="2" width="9" style="9"/>
+    <col min="3" max="3" width="9" style="7"/>
+    <col min="4" max="4" width="9" style="9"/>
+    <col min="5" max="5" width="14.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1149,52 +1142,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="8"/>
-    <col min="6" max="6" width="17.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="7"/>
+    <col min="6" max="6" width="17.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please check default funding values from dropdown menu before manually adding funding information _x000a_" sqref="A1:A1048576" xr:uid="{09457D04-CED0-4649-993D-4FF3340F0594}">
-      <formula1>"USBR, CDWR, CDFW"</formula1>
+      <formula1>"USBR, CDWR, CDFW, USFWS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1210,16 +1203,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1249,17 +1242,17 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1282,28 +1275,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="7"/>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>